<commit_message>
PDS data bugs fixing (#3601)
* diff crush fixing

* fix a bug

Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/ThMEPEngine/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/ThMEPEngine/Contents/Support/平面关注对象.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="528">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2293,9 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3368,9 +3366,6 @@
       </c>
       <c r="C30" t="s">
         <v>227</v>
-      </c>
-      <c r="D30" t="s">
-        <v>232</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>210</v>

</xml_diff>